<commit_message>
copy doi to text working!!!! muahhh.
</commit_message>
<xml_diff>
--- a/searches/sec4_results/outline_4.xlsx
+++ b/searches/sec4_results/outline_4.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N57"/>
+  <dimension ref="A1:L57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -422,74 +434,64 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>SECTION</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>SUBSECTION</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>POINT</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>QUERY</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>DOI</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>PAPER_TITLE</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>RELEVANCE_SCORE</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>FULL_TEXT</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>BIBTEX</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>PDF_LOCATION</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>JOURNAL</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>CITATION_COUNT</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>RANK</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>ADOI_URL</t>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>document_title</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>section_title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>point_text</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>query</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>doi</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>full_text</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>bibtex</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>pdf_location</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>journal</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>citation_count</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>relevance_score</t>
         </is>
       </c>
     </row>
@@ -506,12 +508,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>â€¢ Techniques for data cleaning, outlier detection, and handling missing or inconsistent data in real-time</t>
+          <t>â€¢ The importance of data quality and preprocessing in the automated irrigation management pipeline</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>TITLE-ABS(({inconsistent data} OR {data inconsistency}) AND ({data harmonization} OR {data integration}) AND ({precision irrigation} OR {site-specific irrigation}) AND {cloud platform})</t>
+          <t>TITLE-ABS-KEY(({data quality} OR {data preprocessing}) AND ({automated irrigation} OR {smart irrigation}) AND ({management pipeline} OR {data pipeline} OR {data workflow}))</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -520,16 +522,16 @@
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
-      <c r="K2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N2" t="inlineStr"/>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -544,12 +546,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>â€¢ Techniques for data cleaning, outlier detection, and handling missing or inconsistent data in real-time</t>
+          <t>â€¢ The importance of data quality and preprocessing in the automated irrigation management pipeline</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>TITLE-ABS-KEY(({data cleaning} OR {data cleansing} OR {data scrubbing}) AND ({real-time data} OR {streaming data}) AND ({irrigation system} OR {precision agriculture}))</t>
+          <t>TITLE-ABS-KEY(({data cleaning} OR {data preparation}) AND ({real-time processing} OR {streaming data}) AND ({precision agriculture} OR {precision irrigation} OR {site-specific irrigation}))</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
@@ -558,16 +560,16 @@
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
-      <c r="K3" t="n">
-        <v>0</v>
-      </c>
-      <c r="L3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N3" t="inlineStr"/>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -582,12 +584,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>â€¢ Techniques for data cleaning, outlier detection, and handling missing or inconsistent data in real-time</t>
+          <t>â€¢ The importance of data quality and preprocessing in the automated irrigation management pipeline</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>TITLE-ABS-KEY(({data cleaning} OR {outlier detection} OR {missing data} OR {data inconsistency} OR {data denoising}) AND ({real-time data} OR {streaming data}) AND ({irrigation system} OR {smart irrigation} OR {precision irrigation}))</t>
+          <t>TITLE-ABS-KEY(({data validation} OR {data verification}) AND ({irrigation automation} OR {irrigation control}) AND ({data-driven decision making} OR {machine learning pipeline}))</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
@@ -596,16 +598,16 @@
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
-      <c r="K4" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0</v>
-      </c>
-      <c r="N4" t="inlineStr"/>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -620,12 +622,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>â€¢ Techniques for data cleaning, outlier detection, and handling missing or inconsistent data in real-time</t>
+          <t>â€¢ The importance of data quality and preprocessing in the automated irrigation management pipeline</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>TITLE-ABS-KEY(({data denoising} OR {noise filtering}) AND ({edge computing} OR {fog computing}) AND ({real-time irrigation} OR {smart irrigation}) AND cloud)</t>
+          <t>TITLE-ABS(({noise reduction} OR {data smoothing}) AND ({data preprocessing} OR {data transformation}) AND ({smart irrigation system} OR {IoT-based irrigation}) AND cloud)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
@@ -634,16 +636,16 @@
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
-      <c r="K5" t="n">
-        <v>0</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0</v>
-      </c>
-      <c r="M5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N5" t="inlineStr"/>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -658,12 +660,12 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>â€¢ Techniques for data cleaning, outlier detection, and handling missing or inconsistent data in real-time</t>
+          <t>â€¢ The importance of data quality and preprocessing in the automated irrigation management pipeline</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>TITLE-ABS-KEY(({missing data} OR {data imputation}) AND ({real-time processing} OR {low-latency processing}) AND ({irrigation management} OR {irrigation control}) AND {cloud computing})</t>
+          <t>TITLE-ABS-KEY(({data normalization} OR {feature scaling}) AND ({data quality assurance} OR {data quality management}) AND ({irrigation scheduling} OR {irrigation optimization}) AND {cloud computing})</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
@@ -672,16 +674,16 @@
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr"/>
-      <c r="K6" t="n">
-        <v>0</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N6" t="inlineStr"/>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -696,12 +698,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>â€¢ Techniques for data cleaning, outlier detection, and handling missing or inconsistent data in real-time</t>
+          <t>â€¢ The importance of data quality and preprocessing in the automated irrigation management pipeline</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>TITLE-ABS-KEY(({outlier detection} OR {anomaly detection}) AND ({online learning} OR {incremental learning}) AND ({smart irrigation} OR {IoT-based irrigation}) AND cloud)</t>
+          <t>TITLE-ABS-KEY(({data quality} OR {data preprocessing} OR {data cleaning} OR {data preparation}) AND ({automated irrigation} OR {smart irrigation} OR {precision agriculture} OR {site-specific irrigation}) AND {irrigation management})</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
@@ -710,16 +712,16 @@
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
-      <c r="K7" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" t="n">
-        <v>0</v>
-      </c>
-      <c r="M7" t="n">
-        <v>0</v>
-      </c>
-      <c r="N7" t="inlineStr"/>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -734,12 +736,12 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>â€¢ Techniques for data cleaning, outlier detection, and handling missing or inconsistent data in real-time</t>
+          <t>â€¢ The importance of data quality and preprocessing in the automated irrigation management pipeline</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>TITLE-ABS-KEY({data cleaning} AND {real-time data} AND {irrigation system})</t>
+          <t>TITLE-ABS-KEY({data preprocessing} AND {automated irrigation} AND {management pipeline})</t>
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
@@ -748,16 +750,16 @@
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
-      <c r="K8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L8" t="n">
-        <v>0</v>
-      </c>
-      <c r="M8" t="n">
-        <v>0</v>
-      </c>
-      <c r="N8" t="inlineStr"/>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -772,12 +774,12 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>â€¢ The impact of data quality on the accuracy and reliability of ML models and decision-making processes</t>
+          <t>â€¢ Techniques for data cleaning, outlier detection, and handling missing or inconsistent data in real-time</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>TITLE-ABS(({noisy data} OR {corrupted data} OR {inconsistent data}) AND ({model robustness} OR {model reliability}) AND ({precision irrigation} OR {variable rate irrigation}))</t>
+          <t>TITLE-ABS-KEY(({data cleaning} OR {data cleansing} OR {data scrubbing}) AND ({real-time data} OR {streaming data}) AND ({irrigation system} OR {precision agriculture}))</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
@@ -786,16 +788,16 @@
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
-      <c r="K9" t="n">
-        <v>0</v>
-      </c>
-      <c r="L9" t="n">
-        <v>0</v>
-      </c>
-      <c r="M9" t="n">
-        <v>0</v>
-      </c>
-      <c r="N9" t="inlineStr"/>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -810,12 +812,12 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>â€¢ The impact of data quality on the accuracy and reliability of ML models and decision-making processes</t>
+          <t>â€¢ Techniques for data cleaning, outlier detection, and handling missing or inconsistent data in real-time</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>TITLE-ABS-KEY(({data preprocessing impact} OR {data cleaning effect}) AND ({prediction accuracy} OR {classification performance}) AND ({smart irrigation} OR {IoT-based irrigation}) AND {cloud computing})</t>
+          <t>TITLE-ABS-KEY(({outlier detection} OR {anomaly detection}) AND ({online learning} OR {incremental learning}) AND ({smart irrigation} OR {IoT-based irrigation}) AND cloud)</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
@@ -824,16 +826,16 @@
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
-      <c r="K10" t="n">
-        <v>0</v>
-      </c>
-      <c r="L10" t="n">
-        <v>0</v>
-      </c>
-      <c r="M10" t="n">
-        <v>0</v>
-      </c>
-      <c r="N10" t="inlineStr"/>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -848,12 +850,12 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>â€¢ The impact of data quality on the accuracy and reliability of ML models and decision-making processes</t>
+          <t>â€¢ Techniques for data cleaning, outlier detection, and handling missing or inconsistent data in real-time</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>TITLE-ABS-KEY(({data quality influence} OR {data quality importance}) AND ({decision support system} OR {expert system}) AND ({irrigation scheduling} OR {irrigation control}) AND cloud)</t>
+          <t>TITLE-ABS-KEY(({missing data} OR {data imputation}) AND ({real-time processing} OR {low-latency processing}) AND ({irrigation management} OR {irrigation control}) AND {cloud computing})</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
@@ -862,16 +864,16 @@
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr"/>
-      <c r="K11" t="n">
-        <v>0</v>
-      </c>
-      <c r="L11" t="n">
-        <v>0</v>
-      </c>
-      <c r="M11" t="n">
-        <v>0</v>
-      </c>
-      <c r="N11" t="inlineStr"/>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -886,12 +888,12 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>â€¢ The impact of data quality on the accuracy and reliability of ML models and decision-making processes</t>
+          <t>â€¢ Techniques for data cleaning, outlier detection, and handling missing or inconsistent data in real-time</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>TITLE-ABS-KEY(({data quality metrics} OR {data quality assessment}) AND ({machine learning pipeline} OR {AI workflow}) AND ({irrigation optimization} OR {water productivity}) AND {cloud platform})</t>
+          <t>TITLE-ABS(({inconsistent data} OR {data inconsistency}) AND ({data harmonization} OR {data integration}) AND ({precision irrigation} OR {site-specific irrigation}) AND {cloud platform})</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
@@ -900,16 +902,16 @@
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr"/>
-      <c r="K12" t="n">
-        <v>0</v>
-      </c>
-      <c r="L12" t="n">
-        <v>0</v>
-      </c>
-      <c r="M12" t="n">
-        <v>0</v>
-      </c>
-      <c r="N12" t="inlineStr"/>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -924,12 +926,12 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>â€¢ The impact of data quality on the accuracy and reliability of ML models and decision-making processes</t>
+          <t>â€¢ Techniques for data cleaning, outlier detection, and handling missing or inconsistent data in real-time</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>TITLE-ABS-KEY(({data quality} OR {data preprocessing} OR {data cleaning}) AND ({machine learning} OR {model performance} OR {decision making}) AND ({irrigation management} OR {smart irrigation}))</t>
+          <t>TITLE-ABS-KEY(({data denoising} OR {noise filtering}) AND ({edge computing} OR {fog computing}) AND ({real-time irrigation} OR {smart irrigation}) AND cloud)</t>
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
@@ -938,16 +940,16 @@
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
-      <c r="K13" t="n">
-        <v>0</v>
-      </c>
-      <c r="L13" t="n">
-        <v>0</v>
-      </c>
-      <c r="M13" t="n">
-        <v>0</v>
-      </c>
-      <c r="N13" t="inlineStr"/>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -962,12 +964,12 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>â€¢ The impact of data quality on the accuracy and reliability of ML models and decision-making processes</t>
+          <t>â€¢ Techniques for data cleaning, outlier detection, and handling missing or inconsistent data in real-time</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>TITLE-ABS-KEY(({data quality} OR {data reliability}) AND ({machine learning accuracy} OR {model performance}) AND ({irrigation management} OR {precision agriculture}))</t>
+          <t>TITLE-ABS-KEY(({data cleaning} OR {outlier detection} OR {missing data} OR {data inconsistency} OR {data denoising}) AND ({real-time data} OR {streaming data}) AND ({irrigation system} OR {smart irrigation} OR {precision irrigation}))</t>
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
@@ -976,16 +978,16 @@
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr"/>
-      <c r="K14" t="n">
-        <v>0</v>
-      </c>
-      <c r="L14" t="n">
-        <v>0</v>
-      </c>
-      <c r="M14" t="n">
-        <v>0</v>
-      </c>
-      <c r="N14" t="inlineStr"/>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1000,12 +1002,12 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>â€¢ The impact of data quality on the accuracy and reliability of ML models and decision-making processes</t>
+          <t>â€¢ Techniques for data cleaning, outlier detection, and handling missing or inconsistent data in real-time</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>TITLE-ABS-KEY({data quality} AND {machine learning accuracy} AND {irrigation management})</t>
+          <t>TITLE-ABS-KEY({data cleaning} AND {real-time data} AND {irrigation system})</t>
         </is>
       </c>
       <c r="E15" t="inlineStr"/>
@@ -1014,16 +1016,16 @@
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr"/>
-      <c r="K15" t="n">
-        <v>0</v>
-      </c>
-      <c r="L15" t="n">
-        <v>0</v>
-      </c>
-      <c r="M15" t="n">
-        <v>0</v>
-      </c>
-      <c r="N15" t="inlineStr"/>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1038,12 +1040,12 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>â€¢ The importance of data quality and preprocessing in the automated irrigation management pipeline</t>
+          <t>â€¢ The impact of data quality on the accuracy and reliability of ML models and decision-making processes</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>TITLE-ABS(({noise reduction} OR {data smoothing}) AND ({data preprocessing} OR {data transformation}) AND ({smart irrigation system} OR {IoT-based irrigation}) AND cloud)</t>
+          <t>TITLE-ABS-KEY(({data quality} OR {data reliability}) AND ({machine learning accuracy} OR {model performance}) AND ({irrigation management} OR {precision agriculture}))</t>
         </is>
       </c>
       <c r="E16" t="inlineStr"/>
@@ -1052,16 +1054,16 @@
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr"/>
-      <c r="K16" t="n">
-        <v>0</v>
-      </c>
-      <c r="L16" t="n">
-        <v>0</v>
-      </c>
-      <c r="M16" t="n">
-        <v>0</v>
-      </c>
-      <c r="N16" t="inlineStr"/>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1076,12 +1078,12 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>â€¢ The importance of data quality and preprocessing in the automated irrigation management pipeline</t>
+          <t>â€¢ The impact of data quality on the accuracy and reliability of ML models and decision-making processes</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>TITLE-ABS-KEY(({data cleaning} OR {data preparation}) AND ({real-time processing} OR {streaming data}) AND ({precision agriculture} OR {precision irrigation} OR {site-specific irrigation}))</t>
+          <t>TITLE-ABS-KEY(({data preprocessing impact} OR {data cleaning effect}) AND ({prediction accuracy} OR {classification performance}) AND ({smart irrigation} OR {IoT-based irrigation}) AND {cloud computing})</t>
         </is>
       </c>
       <c r="E17" t="inlineStr"/>
@@ -1090,16 +1092,16 @@
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr"/>
-      <c r="K17" t="n">
-        <v>0</v>
-      </c>
-      <c r="L17" t="n">
-        <v>0</v>
-      </c>
-      <c r="M17" t="n">
-        <v>0</v>
-      </c>
-      <c r="N17" t="inlineStr"/>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1114,12 +1116,12 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>â€¢ The importance of data quality and preprocessing in the automated irrigation management pipeline</t>
+          <t>â€¢ The impact of data quality on the accuracy and reliability of ML models and decision-making processes</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>TITLE-ABS-KEY(({data normalization} OR {feature scaling}) AND ({data quality assurance} OR {data quality management}) AND ({irrigation scheduling} OR {irrigation optimization}) AND {cloud computing})</t>
+          <t>TITLE-ABS-KEY(({data quality influence} OR {data quality importance}) AND ({decision support system} OR {expert system}) AND ({irrigation scheduling} OR {irrigation control}) AND cloud)</t>
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
@@ -1128,16 +1130,16 @@
       <c r="H18" t="inlineStr"/>
       <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr"/>
-      <c r="K18" t="n">
-        <v>0</v>
-      </c>
-      <c r="L18" t="n">
-        <v>0</v>
-      </c>
-      <c r="M18" t="n">
-        <v>0</v>
-      </c>
-      <c r="N18" t="inlineStr"/>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1152,12 +1154,12 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>â€¢ The importance of data quality and preprocessing in the automated irrigation management pipeline</t>
+          <t>â€¢ The impact of data quality on the accuracy and reliability of ML models and decision-making processes</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>TITLE-ABS-KEY(({data quality} OR {data preprocessing} OR {data cleaning} OR {data preparation}) AND ({automated irrigation} OR {smart irrigation} OR {precision agriculture} OR {site-specific irrigation}) AND {irrigation management})</t>
+          <t>TITLE-ABS(({noisy data} OR {corrupted data} OR {inconsistent data}) AND ({model robustness} OR {model reliability}) AND ({precision irrigation} OR {variable rate irrigation}))</t>
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
@@ -1166,16 +1168,16 @@
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr"/>
-      <c r="K19" t="n">
-        <v>0</v>
-      </c>
-      <c r="L19" t="n">
-        <v>0</v>
-      </c>
-      <c r="M19" t="n">
-        <v>0</v>
-      </c>
-      <c r="N19" t="inlineStr"/>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1190,12 +1192,12 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>â€¢ The importance of data quality and preprocessing in the automated irrigation management pipeline</t>
+          <t>â€¢ The impact of data quality on the accuracy and reliability of ML models and decision-making processes</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>TITLE-ABS-KEY(({data quality} OR {data preprocessing}) AND ({automated irrigation} OR {smart irrigation}) AND ({management pipeline} OR {data pipeline} OR {data workflow}))</t>
+          <t>TITLE-ABS-KEY(({data quality metrics} OR {data quality assessment}) AND ({machine learning pipeline} OR {AI workflow}) AND ({irrigation optimization} OR {water productivity}) AND {cloud platform})</t>
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
@@ -1204,16 +1206,16 @@
       <c r="H20" t="inlineStr"/>
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr"/>
-      <c r="K20" t="n">
-        <v>0</v>
-      </c>
-      <c r="L20" t="n">
-        <v>0</v>
-      </c>
-      <c r="M20" t="n">
-        <v>0</v>
-      </c>
-      <c r="N20" t="inlineStr"/>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1228,12 +1230,12 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>â€¢ The importance of data quality and preprocessing in the automated irrigation management pipeline</t>
+          <t>â€¢ The impact of data quality on the accuracy and reliability of ML models and decision-making processes</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>TITLE-ABS-KEY(({data validation} OR {data verification}) AND ({irrigation automation} OR {irrigation control}) AND ({data-driven decision making} OR {machine learning pipeline}))</t>
+          <t>TITLE-ABS-KEY(({data quality} OR {data preprocessing} OR {data cleaning}) AND ({machine learning} OR {model performance} OR {decision making}) AND ({irrigation management} OR {smart irrigation}))</t>
         </is>
       </c>
       <c r="E21" t="inlineStr"/>
@@ -1242,16 +1244,16 @@
       <c r="H21" t="inlineStr"/>
       <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr"/>
-      <c r="K21" t="n">
-        <v>0</v>
-      </c>
-      <c r="L21" t="n">
-        <v>0</v>
-      </c>
-      <c r="M21" t="n">
-        <v>0</v>
-      </c>
-      <c r="N21" t="inlineStr"/>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1266,12 +1268,12 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>â€¢ The importance of data quality and preprocessing in the automated irrigation management pipeline</t>
+          <t>â€¢ The impact of data quality on the accuracy and reliability of ML models and decision-making processes</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>TITLE-ABS-KEY({data preprocessing} AND {automated irrigation} AND {management pipeline})</t>
+          <t>TITLE-ABS-KEY({data quality} AND {machine learning accuracy} AND {irrigation management})</t>
         </is>
       </c>
       <c r="E22" t="inlineStr"/>
@@ -1280,16 +1282,16 @@
       <c r="H22" t="inlineStr"/>
       <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr"/>
-      <c r="K22" t="n">
-        <v>0</v>
-      </c>
-      <c r="L22" t="n">
-        <v>0</v>
-      </c>
-      <c r="M22" t="n">
-        <v>0</v>
-      </c>
-      <c r="N22" t="inlineStr"/>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1304,12 +1306,12 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>â€¢ Benefits and challenges of containerization in the context of real-time irrigation management</t>
+          <t>â€¢ Examination of containerization technologies (e.g., Docker, Kubernetes) for hosting, running, and scaling ML/data processing modules in the cloud</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>TITLE-ABS((containerization AND ({performance overhead} OR {resource utilization})) AND ({real-time decision making} OR {low-latency response}) AND ({precision agriculture} OR {variable rate irrigation}))</t>
+          <t>TITLE-ABS-KEY(({containerization} OR {container technology}) AND ({machine learning deployment} OR {ML pipeline}) AND ({irrigation management} OR {precision agriculture}) AND {cloud computing})</t>
         </is>
       </c>
       <c r="E23" t="inlineStr"/>
@@ -1318,16 +1320,16 @@
       <c r="H23" t="inlineStr"/>
       <c r="I23" t="inlineStr"/>
       <c r="J23" t="inlineStr"/>
-      <c r="K23" t="n">
-        <v>0</v>
-      </c>
-      <c r="L23" t="n">
-        <v>0</v>
-      </c>
-      <c r="M23" t="n">
-        <v>0</v>
-      </c>
-      <c r="N23" t="inlineStr"/>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1342,12 +1344,12 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>â€¢ Benefits and challenges of containerization in the context of real-time irrigation management</t>
+          <t>â€¢ Examination of containerization technologies (e.g., Docker, Kubernetes) for hosting, running, and scaling ML/data processing modules in the cloud</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>TITLE-ABS-KEY(({container isolation} OR {container security}) AND ({irrigation automation} OR {irrigation optimization}) AND ({data processing} OR {data analysis}) AND {cloud platform})</t>
+          <t>TITLE-ABS-KEY((docker OR kubernetes) AND ({data processing modules} OR {data analytics modules}) AND ({smart irrigation} OR {IoT-based irrigation}) AND {cloud platform})</t>
         </is>
       </c>
       <c r="E24" t="inlineStr"/>
@@ -1356,16 +1358,16 @@
       <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr"/>
       <c r="J24" t="inlineStr"/>
-      <c r="K24" t="n">
-        <v>0</v>
-      </c>
-      <c r="L24" t="n">
-        <v>0</v>
-      </c>
-      <c r="M24" t="n">
-        <v>0</v>
-      </c>
-      <c r="N24" t="inlineStr"/>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1380,12 +1382,12 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>â€¢ Benefits and challenges of containerization in the context of real-time irrigation management</t>
+          <t>â€¢ Examination of containerization technologies (e.g., Docker, Kubernetes) for hosting, running, and scaling ML/data processing modules in the cloud</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>TITLE-ABS-KEY(({container migration} OR {container portability}) AND ({irrigation scheduling} OR {irrigation control}) AND ({edge computing} OR {fog computing}) AND cloud)</t>
+          <t>TITLE-ABS-KEY(({container orchestration} OR {container management}) AND ({ML model serving} OR {ML model inference}) AND ({irrigation scheduling} OR {irrigation control}) AND cloud)</t>
         </is>
       </c>
       <c r="E25" t="inlineStr"/>
@@ -1394,16 +1396,16 @@
       <c r="H25" t="inlineStr"/>
       <c r="I25" t="inlineStr"/>
       <c r="J25" t="inlineStr"/>
-      <c r="K25" t="n">
-        <v>0</v>
-      </c>
-      <c r="L25" t="n">
-        <v>0</v>
-      </c>
-      <c r="M25" t="n">
-        <v>0</v>
-      </c>
-      <c r="N25" t="inlineStr"/>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1418,12 +1420,12 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>â€¢ Benefits and challenges of containerization in the context of real-time irrigation management</t>
+          <t>â€¢ Examination of containerization technologies (e.g., Docker, Kubernetes) for hosting, running, and scaling ML/data processing modules in the cloud</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>TITLE-ABS-KEY(({containerization benefits} OR {containerization advantages}) AND ({real-time irrigation} OR {precision irrigation}) AND ({management system} OR {control system}) AND cloud)</t>
+          <t>TITLE-ABS((containerization AND ({scalability} OR {elasticity})) AND ({real-time data processing} OR {streaming data processing}) AND ({precision irrigation} OR {site-specific irrigation}))</t>
         </is>
       </c>
       <c r="E26" t="inlineStr"/>
@@ -1432,16 +1434,16 @@
       <c r="H26" t="inlineStr"/>
       <c r="I26" t="inlineStr"/>
       <c r="J26" t="inlineStr"/>
-      <c r="K26" t="n">
-        <v>0</v>
-      </c>
-      <c r="L26" t="n">
-        <v>0</v>
-      </c>
-      <c r="M26" t="n">
-        <v>0</v>
-      </c>
-      <c r="N26" t="inlineStr"/>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1456,12 +1458,12 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>â€¢ Benefits and challenges of containerization in the context of real-time irrigation management</t>
+          <t>â€¢ Examination of containerization technologies (e.g., Docker, Kubernetes) for hosting, running, and scaling ML/data processing modules in the cloud</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>TITLE-ABS-KEY(({containerization benefits} OR {containerization challenges} OR {container isolation} OR {container security}) AND ({real-time irrigation} OR {smart irrigation} OR {irrigation automation}) AND {cloud})</t>
+          <t>TITLE-ABS-KEY(({lightweight virtualization} OR {OS-level virtualization}) AND ({irrigation data processing} OR {irrigation data analysis}) AND ({cloud native} OR {cloud agnostic}) AND {precision agriculture})</t>
         </is>
       </c>
       <c r="E27" t="inlineStr"/>
@@ -1470,16 +1472,16 @@
       <c r="H27" t="inlineStr"/>
       <c r="I27" t="inlineStr"/>
       <c r="J27" t="inlineStr"/>
-      <c r="K27" t="n">
-        <v>0</v>
-      </c>
-      <c r="L27" t="n">
-        <v>0</v>
-      </c>
-      <c r="M27" t="n">
-        <v>0</v>
-      </c>
-      <c r="N27" t="inlineStr"/>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1494,12 +1496,12 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>â€¢ Benefits and challenges of containerization in the context of real-time irrigation management</t>
+          <t>â€¢ Examination of containerization technologies (e.g., Docker, Kubernetes) for hosting, running, and scaling ML/data processing modules in the cloud</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>TITLE-ABS-KEY(({containerization challenges} OR {containerization issues}) AND ({smart irrigation} OR {IoT-based irrigation}) AND ({real-time data} OR {streaming data}) AND {cloud computing})</t>
+          <t>TITLE-ABS-KEY(({containerization} OR {container technology} OR {container orchestration} OR {container management}) AND ({machine learning} OR {data processing} OR {data analytics}) AND ({irrigation management} OR {smart irrigation}) AND {cloud})</t>
         </is>
       </c>
       <c r="E28" t="inlineStr"/>
@@ -1508,16 +1510,16 @@
       <c r="H28" t="inlineStr"/>
       <c r="I28" t="inlineStr"/>
       <c r="J28" t="inlineStr"/>
-      <c r="K28" t="n">
-        <v>0</v>
-      </c>
-      <c r="L28" t="n">
-        <v>0</v>
-      </c>
-      <c r="M28" t="n">
-        <v>0</v>
-      </c>
-      <c r="N28" t="inlineStr"/>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1532,12 +1534,12 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>â€¢ Benefits and challenges of containerization in the context of real-time irrigation management</t>
+          <t>â€¢ Examination of containerization technologies (e.g., Docker, Kubernetes) for hosting, running, and scaling ML/data processing modules in the cloud</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>TITLE-ABS-KEY({containerization benefits} AND {real-time irrigation} AND {management system} AND cloud)</t>
+          <t>TITLE-ABS-KEY({containerization} AND {machine learning deployment} AND {irrigation management} AND {cloud computing})</t>
         </is>
       </c>
       <c r="E29" t="inlineStr"/>
@@ -1546,16 +1548,16 @@
       <c r="H29" t="inlineStr"/>
       <c r="I29" t="inlineStr"/>
       <c r="J29" t="inlineStr"/>
-      <c r="K29" t="n">
-        <v>0</v>
-      </c>
-      <c r="L29" t="n">
-        <v>0</v>
-      </c>
-      <c r="M29" t="n">
-        <v>0</v>
-      </c>
-      <c r="N29" t="inlineStr"/>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1570,12 +1572,12 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>â€¢ Examination of containerization technologies (e.g., Docker, Kubernetes) for hosting, running, and scaling ML/data processing modules in the cloud</t>
+          <t>â€¢ Benefits and challenges of containerization in the context of real-time irrigation management</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>TITLE-ABS((containerization AND ({scalability} OR {elasticity})) AND ({real-time data processing} OR {streaming data processing}) AND ({precision irrigation} OR {site-specific irrigation}))</t>
+          <t>TITLE-ABS-KEY(({containerization benefits} OR {containerization advantages}) AND ({real-time irrigation} OR {precision irrigation}) AND ({management system} OR {control system}) AND cloud)</t>
         </is>
       </c>
       <c r="E30" t="inlineStr"/>
@@ -1584,16 +1586,16 @@
       <c r="H30" t="inlineStr"/>
       <c r="I30" t="inlineStr"/>
       <c r="J30" t="inlineStr"/>
-      <c r="K30" t="n">
-        <v>0</v>
-      </c>
-      <c r="L30" t="n">
-        <v>0</v>
-      </c>
-      <c r="M30" t="n">
-        <v>0</v>
-      </c>
-      <c r="N30" t="inlineStr"/>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1608,12 +1610,12 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>â€¢ Examination of containerization technologies (e.g., Docker, Kubernetes) for hosting, running, and scaling ML/data processing modules in the cloud</t>
+          <t>â€¢ Benefits and challenges of containerization in the context of real-time irrigation management</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>TITLE-ABS-KEY((docker OR kubernetes) AND ({data processing modules} OR {data analytics modules}) AND ({smart irrigation} OR {IoT-based irrigation}) AND {cloud platform})</t>
+          <t>TITLE-ABS-KEY(({containerization challenges} OR {containerization issues}) AND ({smart irrigation} OR {IoT-based irrigation}) AND ({real-time data} OR {streaming data}) AND {cloud computing})</t>
         </is>
       </c>
       <c r="E31" t="inlineStr"/>
@@ -1622,16 +1624,16 @@
       <c r="H31" t="inlineStr"/>
       <c r="I31" t="inlineStr"/>
       <c r="J31" t="inlineStr"/>
-      <c r="K31" t="n">
-        <v>0</v>
-      </c>
-      <c r="L31" t="n">
-        <v>0</v>
-      </c>
-      <c r="M31" t="n">
-        <v>0</v>
-      </c>
-      <c r="N31" t="inlineStr"/>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1646,12 +1648,12 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>â€¢ Examination of containerization technologies (e.g., Docker, Kubernetes) for hosting, running, and scaling ML/data processing modules in the cloud</t>
+          <t>â€¢ Benefits and challenges of containerization in the context of real-time irrigation management</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>TITLE-ABS-KEY(({container orchestration} OR {container management}) AND ({ML model serving} OR {ML model inference}) AND ({irrigation scheduling} OR {irrigation control}) AND cloud)</t>
+          <t>TITLE-ABS-KEY(({container isolation} OR {container security}) AND ({irrigation automation} OR {irrigation optimization}) AND ({data processing} OR {data analysis}) AND {cloud platform})</t>
         </is>
       </c>
       <c r="E32" t="inlineStr"/>
@@ -1660,16 +1662,16 @@
       <c r="H32" t="inlineStr"/>
       <c r="I32" t="inlineStr"/>
       <c r="J32" t="inlineStr"/>
-      <c r="K32" t="n">
-        <v>0</v>
-      </c>
-      <c r="L32" t="n">
-        <v>0</v>
-      </c>
-      <c r="M32" t="n">
-        <v>0</v>
-      </c>
-      <c r="N32" t="inlineStr"/>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1684,12 +1686,12 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>â€¢ Examination of containerization technologies (e.g., Docker, Kubernetes) for hosting, running, and scaling ML/data processing modules in the cloud</t>
+          <t>â€¢ Benefits and challenges of containerization in the context of real-time irrigation management</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>TITLE-ABS-KEY(({containerization} OR {container technology} OR {container orchestration} OR {container management}) AND ({machine learning} OR {data processing} OR {data analytics}) AND ({irrigation management} OR {smart irrigation}) AND {cloud})</t>
+          <t>TITLE-ABS((containerization AND ({performance overhead} OR {resource utilization})) AND ({real-time decision making} OR {low-latency response}) AND ({precision agriculture} OR {variable rate irrigation}))</t>
         </is>
       </c>
       <c r="E33" t="inlineStr"/>
@@ -1698,16 +1700,16 @@
       <c r="H33" t="inlineStr"/>
       <c r="I33" t="inlineStr"/>
       <c r="J33" t="inlineStr"/>
-      <c r="K33" t="n">
-        <v>0</v>
-      </c>
-      <c r="L33" t="n">
-        <v>0</v>
-      </c>
-      <c r="M33" t="n">
-        <v>0</v>
-      </c>
-      <c r="N33" t="inlineStr"/>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1722,12 +1724,12 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>â€¢ Examination of containerization technologies (e.g., Docker, Kubernetes) for hosting, running, and scaling ML/data processing modules in the cloud</t>
+          <t>â€¢ Benefits and challenges of containerization in the context of real-time irrigation management</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>TITLE-ABS-KEY(({containerization} OR {container technology}) AND ({machine learning deployment} OR {ML pipeline}) AND ({irrigation management} OR {precision agriculture}) AND {cloud computing})</t>
+          <t>TITLE-ABS-KEY(({container migration} OR {container portability}) AND ({irrigation scheduling} OR {irrigation control}) AND ({edge computing} OR {fog computing}) AND cloud)</t>
         </is>
       </c>
       <c r="E34" t="inlineStr"/>
@@ -1736,16 +1738,16 @@
       <c r="H34" t="inlineStr"/>
       <c r="I34" t="inlineStr"/>
       <c r="J34" t="inlineStr"/>
-      <c r="K34" t="n">
-        <v>0</v>
-      </c>
-      <c r="L34" t="n">
-        <v>0</v>
-      </c>
-      <c r="M34" t="n">
-        <v>0</v>
-      </c>
-      <c r="N34" t="inlineStr"/>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1760,12 +1762,12 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>â€¢ Examination of containerization technologies (e.g., Docker, Kubernetes) for hosting, running, and scaling ML/data processing modules in the cloud</t>
+          <t>â€¢ Benefits and challenges of containerization in the context of real-time irrigation management</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>TITLE-ABS-KEY(({lightweight virtualization} OR {OS-level virtualization}) AND ({irrigation data processing} OR {irrigation data analysis}) AND ({cloud native} OR {cloud agnostic}) AND {precision agriculture})</t>
+          <t>TITLE-ABS-KEY(({containerization benefits} OR {containerization challenges} OR {container isolation} OR {container security}) AND ({real-time irrigation} OR {smart irrigation} OR {irrigation automation}) AND {cloud})</t>
         </is>
       </c>
       <c r="E35" t="inlineStr"/>
@@ -1774,16 +1776,16 @@
       <c r="H35" t="inlineStr"/>
       <c r="I35" t="inlineStr"/>
       <c r="J35" t="inlineStr"/>
-      <c r="K35" t="n">
-        <v>0</v>
-      </c>
-      <c r="L35" t="n">
-        <v>0</v>
-      </c>
-      <c r="M35" t="n">
-        <v>0</v>
-      </c>
-      <c r="N35" t="inlineStr"/>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1798,12 +1800,12 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>â€¢ Examination of containerization technologies (e.g., Docker, Kubernetes) for hosting, running, and scaling ML/data processing modules in the cloud</t>
+          <t>â€¢ Benefits and challenges of containerization in the context of real-time irrigation management</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>TITLE-ABS-KEY({containerization} AND {machine learning deployment} AND {irrigation management} AND {cloud computing})</t>
+          <t>TITLE-ABS-KEY({containerization benefits} AND {real-time irrigation} AND {management system} AND cloud)</t>
         </is>
       </c>
       <c r="E36" t="inlineStr"/>
@@ -1812,16 +1814,16 @@
       <c r="H36" t="inlineStr"/>
       <c r="I36" t="inlineStr"/>
       <c r="J36" t="inlineStr"/>
-      <c r="K36" t="n">
-        <v>0</v>
-      </c>
-      <c r="L36" t="n">
-        <v>0</v>
-      </c>
-      <c r="M36" t="n">
-        <v>0</v>
-      </c>
-      <c r="N36" t="inlineStr"/>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1841,7 +1843,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>TITLE-ABS(({map-reduce} OR {Apache Spark}) AND ({big data processing} OR {large-scale data analysis}) AND ({precision irrigation} OR {site-specific irrigation}) AND {cloud environment})</t>
+          <t>TITLE-ABS-KEY(({parallel processing} OR {distributed computing}) AND ({performance optimization} OR {scalability enhancement}) AND ({irrigation management} OR {precision agriculture}) AND {cloud computing})</t>
         </is>
       </c>
       <c r="E37" t="inlineStr"/>
@@ -1850,16 +1852,16 @@
       <c r="H37" t="inlineStr"/>
       <c r="I37" t="inlineStr"/>
       <c r="J37" t="inlineStr"/>
-      <c r="K37" t="n">
-        <v>0</v>
-      </c>
-      <c r="L37" t="n">
-        <v>0</v>
-      </c>
-      <c r="M37" t="n">
-        <v>0</v>
-      </c>
-      <c r="N37" t="inlineStr"/>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1879,7 +1881,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>TITLE-ABS-KEY(({auto-scaling} OR {dynamic scaling}) AND ({resource optimization} OR {cost optimization}) AND ({irrigation automation} OR {irrigation optimization}) AND {cloud services})</t>
+          <t>TITLE-ABS-KEY(({resource allocation} OR {resource provisioning}) AND ({load balancing} OR {workload distribution}) AND ({smart irrigation} OR {IoT-based irrigation}) AND {cloud platform})</t>
         </is>
       </c>
       <c r="E38" t="inlineStr"/>
@@ -1888,16 +1890,16 @@
       <c r="H38" t="inlineStr"/>
       <c r="I38" t="inlineStr"/>
       <c r="J38" t="inlineStr"/>
-      <c r="K38" t="n">
-        <v>0</v>
-      </c>
-      <c r="L38" t="n">
-        <v>0</v>
-      </c>
-      <c r="M38" t="n">
-        <v>0</v>
-      </c>
-      <c r="N38" t="inlineStr"/>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1926,16 +1928,16 @@
       <c r="H39" t="inlineStr"/>
       <c r="I39" t="inlineStr"/>
       <c r="J39" t="inlineStr"/>
-      <c r="K39" t="n">
-        <v>0</v>
-      </c>
-      <c r="L39" t="n">
-        <v>0</v>
-      </c>
-      <c r="M39" t="n">
-        <v>0</v>
-      </c>
-      <c r="N39" t="inlineStr"/>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1955,7 +1957,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>TITLE-ABS-KEY(({parallel processing} OR {distributed computing} OR {resource allocation} OR {horizontal scaling} OR {auto-scaling}) AND ({performance optimization} OR {scalability enhancement}) AND ({irrigation management} OR {smart irrigation}) AND {cloud})</t>
+          <t>TITLE-ABS(({map-reduce} OR {Apache Spark}) AND ({big data processing} OR {large-scale data analysis}) AND ({precision irrigation} OR {site-specific irrigation}) AND {cloud environment})</t>
         </is>
       </c>
       <c r="E40" t="inlineStr"/>
@@ -1964,16 +1966,16 @@
       <c r="H40" t="inlineStr"/>
       <c r="I40" t="inlineStr"/>
       <c r="J40" t="inlineStr"/>
-      <c r="K40" t="n">
-        <v>0</v>
-      </c>
-      <c r="L40" t="n">
-        <v>0</v>
-      </c>
-      <c r="M40" t="n">
-        <v>0</v>
-      </c>
-      <c r="N40" t="inlineStr"/>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1993,7 +1995,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>TITLE-ABS-KEY(({parallel processing} OR {distributed computing}) AND ({performance optimization} OR {scalability enhancement}) AND ({irrigation management} OR {precision agriculture}) AND {cloud computing})</t>
+          <t>TITLE-ABS-KEY(({auto-scaling} OR {dynamic scaling}) AND ({resource optimization} OR {cost optimization}) AND ({irrigation automation} OR {irrigation optimization}) AND {cloud services})</t>
         </is>
       </c>
       <c r="E41" t="inlineStr"/>
@@ -2002,16 +2004,16 @@
       <c r="H41" t="inlineStr"/>
       <c r="I41" t="inlineStr"/>
       <c r="J41" t="inlineStr"/>
-      <c r="K41" t="n">
-        <v>0</v>
-      </c>
-      <c r="L41" t="n">
-        <v>0</v>
-      </c>
-      <c r="M41" t="n">
-        <v>0</v>
-      </c>
-      <c r="N41" t="inlineStr"/>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -2031,7 +2033,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>TITLE-ABS-KEY(({resource allocation} OR {resource provisioning}) AND ({load balancing} OR {workload distribution}) AND ({smart irrigation} OR {IoT-based irrigation}) AND {cloud platform})</t>
+          <t>TITLE-ABS-KEY(({parallel processing} OR {distributed computing} OR {resource allocation} OR {horizontal scaling} OR {auto-scaling}) AND ({performance optimization} OR {scalability enhancement}) AND ({irrigation management} OR {smart irrigation}) AND {cloud})</t>
         </is>
       </c>
       <c r="E42" t="inlineStr"/>
@@ -2040,16 +2042,16 @@
       <c r="H42" t="inlineStr"/>
       <c r="I42" t="inlineStr"/>
       <c r="J42" t="inlineStr"/>
-      <c r="K42" t="n">
-        <v>0</v>
-      </c>
-      <c r="L42" t="n">
-        <v>0</v>
-      </c>
-      <c r="M42" t="n">
-        <v>0</v>
-      </c>
-      <c r="N42" t="inlineStr"/>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2078,16 +2080,16 @@
       <c r="H43" t="inlineStr"/>
       <c r="I43" t="inlineStr"/>
       <c r="J43" t="inlineStr"/>
-      <c r="K43" t="n">
-        <v>0</v>
-      </c>
-      <c r="L43" t="n">
-        <v>0</v>
-      </c>
-      <c r="M43" t="n">
-        <v>0</v>
-      </c>
-      <c r="N43" t="inlineStr"/>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2107,7 +2109,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>TITLE-ABS(({model scoring} OR {model prediction}) AND ({RESTful API} OR {gRPC API}) AND ({precision irrigation} OR {site-specific irrigation}) AND {cloud environment})</t>
+          <t>TITLE-ABS-KEY(({machine learning deployment} OR {ML model deployment}) AND ({cloud platform} OR {cloud service}) AND ({real-time data processing} OR {streaming data processing}) AND ({irrigation management} OR {precision agriculture}))</t>
         </is>
       </c>
       <c r="E44" t="inlineStr"/>
@@ -2116,16 +2118,16 @@
       <c r="H44" t="inlineStr"/>
       <c r="I44" t="inlineStr"/>
       <c r="J44" t="inlineStr"/>
-      <c r="K44" t="n">
-        <v>0</v>
-      </c>
-      <c r="L44" t="n">
-        <v>0</v>
-      </c>
-      <c r="M44" t="n">
-        <v>0</v>
-      </c>
-      <c r="N44" t="inlineStr"/>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -2154,16 +2156,16 @@
       <c r="H45" t="inlineStr"/>
       <c r="I45" t="inlineStr"/>
       <c r="J45" t="inlineStr"/>
-      <c r="K45" t="n">
-        <v>0</v>
-      </c>
-      <c r="L45" t="n">
-        <v>0</v>
-      </c>
-      <c r="M45" t="n">
-        <v>0</v>
-      </c>
-      <c r="N45" t="inlineStr"/>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2192,16 +2194,16 @@
       <c r="H46" t="inlineStr"/>
       <c r="I46" t="inlineStr"/>
       <c r="J46" t="inlineStr"/>
-      <c r="K46" t="n">
-        <v>0</v>
-      </c>
-      <c r="L46" t="n">
-        <v>0</v>
-      </c>
-      <c r="M46" t="n">
-        <v>0</v>
-      </c>
-      <c r="N46" t="inlineStr"/>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2221,7 +2223,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>TITLE-ABS-KEY(({machine learning deployment} OR {ML model deployment} OR {ML pipeline} OR {model scoring}) AND ({cloud platform} OR {cloud service}) AND ({real-time data processing} OR {streaming data processing}) AND ({irrigation management} OR {smart irrigation}))</t>
+          <t>TITLE-ABS(({model scoring} OR {model prediction}) AND ({RESTful API} OR {gRPC API}) AND ({precision irrigation} OR {site-specific irrigation}) AND {cloud environment})</t>
         </is>
       </c>
       <c r="E47" t="inlineStr"/>
@@ -2230,16 +2232,16 @@
       <c r="H47" t="inlineStr"/>
       <c r="I47" t="inlineStr"/>
       <c r="J47" t="inlineStr"/>
-      <c r="K47" t="n">
-        <v>0</v>
-      </c>
-      <c r="L47" t="n">
-        <v>0</v>
-      </c>
-      <c r="M47" t="n">
-        <v>0</v>
-      </c>
-      <c r="N47" t="inlineStr"/>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -2259,7 +2261,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>TITLE-ABS-KEY(({machine learning deployment} OR {ML model deployment}) AND ({cloud platform} OR {cloud service}) AND ({real-time data processing} OR {streaming data processing}) AND ({irrigation management} OR {precision agriculture}))</t>
+          <t>TITLE-ABS-KEY(({model monitoring} OR {model management}) AND ({cloud DevOps} OR {MLOps}) AND ({irrigation automation} OR {irrigation optimization}) AND ({real-time data} OR {streaming data}))</t>
         </is>
       </c>
       <c r="E48" t="inlineStr"/>
@@ -2268,16 +2270,16 @@
       <c r="H48" t="inlineStr"/>
       <c r="I48" t="inlineStr"/>
       <c r="J48" t="inlineStr"/>
-      <c r="K48" t="n">
-        <v>0</v>
-      </c>
-      <c r="L48" t="n">
-        <v>0</v>
-      </c>
-      <c r="M48" t="n">
-        <v>0</v>
-      </c>
-      <c r="N48" t="inlineStr"/>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2297,7 +2299,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>TITLE-ABS-KEY(({model monitoring} OR {model management}) AND ({cloud DevOps} OR {MLOps}) AND ({irrigation automation} OR {irrigation optimization}) AND ({real-time data} OR {streaming data}))</t>
+          <t>TITLE-ABS-KEY(({machine learning deployment} OR {ML model deployment} OR {ML pipeline} OR {model scoring}) AND ({cloud platform} OR {cloud service}) AND ({real-time data processing} OR {streaming data processing}) AND ({irrigation management} OR {smart irrigation}))</t>
         </is>
       </c>
       <c r="E49" t="inlineStr"/>
@@ -2306,16 +2308,16 @@
       <c r="H49" t="inlineStr"/>
       <c r="I49" t="inlineStr"/>
       <c r="J49" t="inlineStr"/>
-      <c r="K49" t="n">
-        <v>0</v>
-      </c>
-      <c r="L49" t="n">
-        <v>0</v>
-      </c>
-      <c r="M49" t="n">
-        <v>0</v>
-      </c>
-      <c r="N49" t="inlineStr"/>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2344,16 +2346,16 @@
       <c r="H50" t="inlineStr"/>
       <c r="I50" t="inlineStr"/>
       <c r="J50" t="inlineStr"/>
-      <c r="K50" t="n">
-        <v>0</v>
-      </c>
-      <c r="L50" t="n">
-        <v>0</v>
-      </c>
-      <c r="M50" t="n">
-        <v>0</v>
-      </c>
-      <c r="N50" t="inlineStr"/>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -2373,7 +2375,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>TITLE-ABS(({online learning algorithm} OR {incremental learning algorithm}) AND ({performance improvement} OR {accuracy enhancement}) AND ({precision irrigation} OR {site-specific irrigation}) AND {cloud environment})</t>
+          <t>TITLE-ABS-KEY(({online learning} OR {incremental learning}) AND ({continuous improvement} OR {adaptive learning}) AND ({irrigation management} OR {precision agriculture}) AND {cloud computing})</t>
         </is>
       </c>
       <c r="E51" t="inlineStr"/>
@@ -2382,16 +2384,16 @@
       <c r="H51" t="inlineStr"/>
       <c r="I51" t="inlineStr"/>
       <c r="J51" t="inlineStr"/>
-      <c r="K51" t="n">
-        <v>0</v>
-      </c>
-      <c r="L51" t="n">
-        <v>0</v>
-      </c>
-      <c r="M51" t="n">
-        <v>0</v>
-      </c>
-      <c r="N51" t="inlineStr"/>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2411,7 +2413,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>TITLE-ABS-KEY(({concept drift detection} OR {model drift detection}) AND ({model retraining} OR {model fine-tuning}) AND ({irrigation scheduling} OR {irrigation control}) AND cloud)</t>
+          <t>TITLE-ABS-KEY(({real-time model update} OR {dynamic model update}) AND ({incoming data} OR {streaming data}) AND ({smart irrigation} OR {IoT-based irrigation}) AND {cloud platform})</t>
         </is>
       </c>
       <c r="E52" t="inlineStr"/>
@@ -2420,16 +2422,16 @@
       <c r="H52" t="inlineStr"/>
       <c r="I52" t="inlineStr"/>
       <c r="J52" t="inlineStr"/>
-      <c r="K52" t="n">
-        <v>0</v>
-      </c>
-      <c r="L52" t="n">
-        <v>0</v>
-      </c>
-      <c r="M52" t="n">
-        <v>0</v>
-      </c>
-      <c r="N52" t="inlineStr"/>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -2449,7 +2451,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>TITLE-ABS-KEY(({lifelong learning} OR {continual learning}) AND ({knowledge accumulation} OR {knowledge transfer}) AND ({irrigation automation} OR {irrigation optimization}) AND {cloud computing})</t>
+          <t>TITLE-ABS-KEY(({concept drift detection} OR {model drift detection}) AND ({model retraining} OR {model fine-tuning}) AND ({irrigation scheduling} OR {irrigation control}) AND cloud)</t>
         </is>
       </c>
       <c r="E53" t="inlineStr"/>
@@ -2458,16 +2460,16 @@
       <c r="H53" t="inlineStr"/>
       <c r="I53" t="inlineStr"/>
       <c r="J53" t="inlineStr"/>
-      <c r="K53" t="n">
-        <v>0</v>
-      </c>
-      <c r="L53" t="n">
-        <v>0</v>
-      </c>
-      <c r="M53" t="n">
-        <v>0</v>
-      </c>
-      <c r="N53" t="inlineStr"/>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -2487,7 +2489,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>TITLE-ABS-KEY(({online learning} OR {incremental learning} OR {real-time model update} OR {concept drift detection}) AND ({continuous improvement} OR {model retraining} OR {performance improvement}) AND ({irrigation management} OR {smart irrigation}) AND {cloud})</t>
+          <t>TITLE-ABS(({online learning algorithm} OR {incremental learning algorithm}) AND ({performance improvement} OR {accuracy enhancement}) AND ({precision irrigation} OR {site-specific irrigation}) AND {cloud environment})</t>
         </is>
       </c>
       <c r="E54" t="inlineStr"/>
@@ -2496,16 +2498,16 @@
       <c r="H54" t="inlineStr"/>
       <c r="I54" t="inlineStr"/>
       <c r="J54" t="inlineStr"/>
-      <c r="K54" t="n">
-        <v>0</v>
-      </c>
-      <c r="L54" t="n">
-        <v>0</v>
-      </c>
-      <c r="M54" t="n">
-        <v>0</v>
-      </c>
-      <c r="N54" t="inlineStr"/>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L54" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -2525,7 +2527,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>TITLE-ABS-KEY(({online learning} OR {incremental learning}) AND ({continuous improvement} OR {adaptive learning}) AND ({irrigation management} OR {precision agriculture}) AND {cloud computing})</t>
+          <t>TITLE-ABS-KEY(({lifelong learning} OR {continual learning}) AND ({knowledge accumulation} OR {knowledge transfer}) AND ({irrigation automation} OR {irrigation optimization}) AND {cloud computing})</t>
         </is>
       </c>
       <c r="E55" t="inlineStr"/>
@@ -2534,16 +2536,16 @@
       <c r="H55" t="inlineStr"/>
       <c r="I55" t="inlineStr"/>
       <c r="J55" t="inlineStr"/>
-      <c r="K55" t="n">
-        <v>0</v>
-      </c>
-      <c r="L55" t="n">
-        <v>0</v>
-      </c>
-      <c r="M55" t="n">
-        <v>0</v>
-      </c>
-      <c r="N55" t="inlineStr"/>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -2563,7 +2565,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>TITLE-ABS-KEY(({real-time model update} OR {dynamic model update}) AND ({incoming data} OR {streaming data}) AND ({smart irrigation} OR {IoT-based irrigation}) AND {cloud platform})</t>
+          <t>TITLE-ABS-KEY(({online learning} OR {incremental learning} OR {real-time model update} OR {concept drift detection}) AND ({continuous improvement} OR {model retraining} OR {performance improvement}) AND ({irrigation management} OR {smart irrigation}) AND {cloud})</t>
         </is>
       </c>
       <c r="E56" t="inlineStr"/>
@@ -2572,16 +2574,16 @@
       <c r="H56" t="inlineStr"/>
       <c r="I56" t="inlineStr"/>
       <c r="J56" t="inlineStr"/>
-      <c r="K56" t="n">
-        <v>0</v>
-      </c>
-      <c r="L56" t="n">
-        <v>0</v>
-      </c>
-      <c r="M56" t="n">
-        <v>0</v>
-      </c>
-      <c r="N56" t="inlineStr"/>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -2610,16 +2612,16 @@
       <c r="H57" t="inlineStr"/>
       <c r="I57" t="inlineStr"/>
       <c r="J57" t="inlineStr"/>
-      <c r="K57" t="n">
-        <v>0</v>
-      </c>
-      <c r="L57" t="n">
-        <v>0</v>
-      </c>
-      <c r="M57" t="n">
-        <v>0</v>
-      </c>
-      <c r="N57" t="inlineStr"/>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>